<commit_message>
Reupload for A1-A2 and Add evidence for B1-B2
</commit_message>
<xml_diff>
--- a/nurtagum/evidence.xlsx
+++ b/nurtagum/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\1W_nurtagum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0K_nurtagum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA5B2EE-76D8-4F04-BE41-C220B28CF989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DB5025-B067-4A90-8D8E-8115CC610126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="839" firstSheet="2" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t>TxHash</t>
   </si>
@@ -124,46 +124,70 @@
     <t>uptick10sqe94d2l7eu8v7kg57lkuhq3c8mhxrzvk3f42</t>
   </si>
   <si>
-    <t>B3D86011AED38E4FB387ED185BAA69419CC248B614A3FC5CBA75D55C0D739463</t>
-  </si>
-  <si>
-    <t>nrtgm</t>
-  </si>
-  <si>
-    <t>9F55D0EF12161F771FE51B9884826499CCB1EF0B44F29208B47472B79BECB1B5</t>
-  </si>
-  <si>
-    <t>nrtgm1</t>
-  </si>
-  <si>
-    <t>nrtgm2</t>
-  </si>
-  <si>
-    <t>296105D2D4992D19121D1C61CB2980262658A3EA6E06065FBC34DFAE93D56612</t>
-  </si>
-  <si>
-    <t>943744344AC1DE67C08DCCA57631C81D4C38B4E527942A418BE0EDB7125663F7</t>
-  </si>
-  <si>
     <t>elgafar-1</t>
   </si>
   <si>
     <t>gon-flixnet-1</t>
   </si>
   <si>
-    <t>stars1x0074g845vh6t6jdzajwxcgfsfr6lrnllwfzgdavhjm0tmnaewvqec7zyh</t>
-  </si>
-  <si>
-    <t>D11FACEB2841F212789F14EA403B1CC6BEA3C72C45CBF0D311AE7D4106125A42</t>
-  </si>
-  <si>
-    <t>ibc/CB2784F6EC6F94C05E6BB5CABEDACD81ED1117290B3F3B756921A176F8E5D1CB</t>
-  </si>
-  <si>
-    <t>547BED96AC72F8701A53E84C9383AF153E24C6C90D2A28F20AA3F6AFF2408491</t>
-  </si>
-  <si>
-    <t>C7DBC37A22CB87F38484F417F0DA91BE45A85D6715638A2B9FD1AC2ED7DF0ECD</t>
+    <t>BDA296409A227E80211CD9F3DCA8796F4494D103549E1F4400917EE6BD7B60CC</t>
+  </si>
+  <si>
+    <t>nurtagumtwo</t>
+  </si>
+  <si>
+    <t>nurtagumtwo2</t>
+  </si>
+  <si>
+    <t>nurtagumtwo1</t>
+  </si>
+  <si>
+    <t>6D93F47854D3587455A9F30ACC761216FBEFBB81D3C5231CFB6E14059C49079C</t>
+  </si>
+  <si>
+    <t>26EDCFC534BE08498C9E3815D9DE434B45A97EEAD4E2405352A710C6330FFD91</t>
+  </si>
+  <si>
+    <t>nurtagumtwo3</t>
+  </si>
+  <si>
+    <t>4F433D11D336E64DBFFB4B558FDA5501A0A7834638395791AF536268BB66DB8C</t>
+  </si>
+  <si>
+    <t>nurtagumtwo7</t>
+  </si>
+  <si>
+    <t>F0340E470B9B27D49A4849BA9CA3E23B91DF927B7BF2A3739D266369BFB831DE</t>
+  </si>
+  <si>
+    <t>stars1u6lf4wzchcae9ewd9qkj42e06ld7hhytjyg6gpjwzcj75958ljxsy8lknh</t>
+  </si>
+  <si>
+    <t>19E9D052C20E52AB7D13CAC1DD3636FD558D28D6D7D056EF0F7A333EEA9788E6</t>
+  </si>
+  <si>
+    <t>AA2CBE9C65E68697A149043BCB5300E488B157EDA636F696F1791F180F9A0950</t>
+  </si>
+  <si>
+    <t>9C08D588548A5F4AAEDA742565085F30415E468CDDFFC19C34BD2824871F9357</t>
+  </si>
+  <si>
+    <t>ibc/49BD0EAFEA33A732F56ADE90D672067DDB32ABD0E0460B9D8E9EE1CB8443626A</t>
+  </si>
+  <si>
+    <t>D201DF99308507A0E6443C325408C3302AEE9DA3E7CE37BB27FB51E32728FCD9</t>
+  </si>
+  <si>
+    <t>2D29677BC04846395EC17776AA63387CB84C3FC60592F497C25A36F7475CEFF1</t>
+  </si>
+  <si>
+    <t>574A0B8B77DDD6BDEF3F30DDBF9023D4113E43761AEF78A33E9446AC6FAF0701</t>
+  </si>
+  <si>
+    <t>7A4AE23FB5396B3723250DF1B227E8255088C9EC2A5450C531CA051D0DF2E60D</t>
+  </si>
+  <si>
+    <t>57F7DF354D3983BCA603222B4FEAFCB3DDEE33EF5F976FA9377C3FAA6D259E90</t>
   </si>
 </sst>
 </file>
@@ -567,7 +591,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1101,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,10 +1119,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1209,6 +1233,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1236,8 +1332,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1270,83 +1366,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,25 +1396,83 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1428,16 +1514,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1479,16 +1565,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1504,7 +1590,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,16 +1616,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1554,8 +1640,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,16 +1668,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1606,7 +1692,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
add evidence for A7-A20
</commit_message>
<xml_diff>
--- a/nurtagum/evidence.xlsx
+++ b/nurtagum/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0K_nurtagum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0K_nurtagum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DB5025-B067-4A90-8D8E-8115CC610126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C9FDF-D087-4962-B4C5-EE99485DA1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="839" firstSheet="2" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -188,13 +173,163 @@
   </si>
   <si>
     <t>57F7DF354D3983BCA603222B4FEAFCB3DDEE33EF5F976FA9377C3FAA6D259E90</t>
+  </si>
+  <si>
+    <t>ibc/E9FC6519E1EC52A525E09567A410D03BE986CA3429EE6592448010CBC8F297AD</t>
+  </si>
+  <si>
+    <t>ibc/D3DA4E88E3B9659C7F0C5711FC7DC9DCB6C7E68FCC229DAD4C2504EEFC901080</t>
+  </si>
+  <si>
+    <t>nurtagumtwo8</t>
+  </si>
+  <si>
+    <t>ibc/04C7CA3CBEF76B171A0620F05F81EB2E1DF1B66005BE88553FBE4003BA043059</t>
+  </si>
+  <si>
+    <t>nurtagumtwo9</t>
+  </si>
+  <si>
+    <t>ibc/32B7A66FA426551BBDB4AB3147EA122620A73F27B581A61D62001CAA3EB30DDA</t>
+  </si>
+  <si>
+    <t>nurtagumtwo10</t>
+  </si>
+  <si>
+    <t>ibc/65A921DEF28341EFAB51657EE34091188CB2FBEF10A8FE2BCC39B78335A54224</t>
+  </si>
+  <si>
+    <t>nurtagumtwo11</t>
+  </si>
+  <si>
+    <t>ibc/57F4D418E7AE184D6904C20064359B0BE5CBFB81D473B0FD80B5B1335A5170CC</t>
+  </si>
+  <si>
+    <t>nurtagumtwo12</t>
+  </si>
+  <si>
+    <t>23734E72A9457A572B3C3B374DD63FB4D17E0D03D4768B74382ACB6E2ACC4D46</t>
+  </si>
+  <si>
+    <t>7026A3EB29D222665CB2B954C4C130116E66BB907F141D0D8F3AF8F20B87BE1B</t>
+  </si>
+  <si>
+    <t>2670EDF2503D2A2FADF0E13EDDB24F8BEC7D1DB1B406E79E6FD176B48EFBF152</t>
+  </si>
+  <si>
+    <t>406C166D26DCEE9A9B26AE894BEF2263730D8CF59ECFFF19B2AA5D2169207CC5</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>23AD686061E34699507F9A3F76CF2DEE7AA59CA42A5B7F5F694162216C6F48E3</t>
+  </si>
+  <si>
+    <t>8BAB62B86DE7BD04FD745EBD9BF0B6CE911873A000319D1ABA0C003E8CA09C13</t>
+  </si>
+  <si>
+    <t>5A48E194A50DF1B39ECC2A3C22C0FAB2CC3F43AF70669454DF27AB698D3F0F30</t>
+  </si>
+  <si>
+    <t>1139E81D631E75D51EC6577B84F20B315DFF2FAAD77DCD175E0B5EE30E748AFA</t>
+  </si>
+  <si>
+    <t>1602E472FD2F2E9171BD6B4B37AC7225DFCCD47173F22C7D5D026C8C97595DD6</t>
+  </si>
+  <si>
+    <t>B9AC82CB2AB568481883B39AA7E29AB3608A468B5BB878E85D2C3B6AEDF2D494</t>
+  </si>
+  <si>
+    <t>0D8689C599D3F478B088489EC2F37987ECB4BC54FF0DBC32D1337717CB7DF27F</t>
+  </si>
+  <si>
+    <t>4FB2B65ABE2081005F62BB1E6DDF73EC02283D184D4DC8706AEAF44CFFEAF60E</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>7097C6C1B20F391884EBE06D694BC42C25700E4694B01E6D9A12009655220923</t>
+  </si>
+  <si>
+    <t>1081CD3C3AD6A10D1D7B85A7079F139D0F57DE00291C0AA5D6651C0181798143</t>
+  </si>
+  <si>
+    <t>A74AACF2D147C3373D507493D972A29A9758FE4542079EB4895A6D99ADFDCDCB</t>
+  </si>
+  <si>
+    <t>FC05AB7138F55C2CC7746F6A0EA82C4A2F3563A068777CD0CED3210FD90CABAC</t>
+  </si>
+  <si>
+    <t>353485C5DB3C0976DFC4D9E2B187A482ACA596E61F9AAFEFDE120535807E2556</t>
+  </si>
+  <si>
+    <t>664E654DB003A983073F8BFFA1D03C1A9AFED40A9346E0EA148B021314632257</t>
+  </si>
+  <si>
+    <t>4A49B6537F2B834BD2917D54FBA72801F8253B4958B51055B7FB4F412C14A969</t>
+  </si>
+  <si>
+    <t>9B9A9E099FD5715EF40D5B93210D13177726A286BF901F128DD72FE4D30162AE</t>
+  </si>
+  <si>
+    <t>4A995F60D3D2A838BC781A708084F8BD12B4EC778EAA41CE32731BC4669B60E5</t>
+  </si>
+  <si>
+    <t>9D7EA735E7C9C8B0EFE94D4F3F5BFB51EB61562C798777028E775DB7EC8043F7</t>
+  </si>
+  <si>
+    <t>8EC1705A68E8F428580A0A6C9C08C683F6EC183E38225015D8797AC188892E4A</t>
+  </si>
+  <si>
+    <t>3A4A1E3787CEDAC190EE23B08FD4965F35E40E456B356C38E7606A460FF15265</t>
+  </si>
+  <si>
+    <t>EA2B1B255DA602F0AD76889E763DCAE03519FBA080952219788890448EC1DC67</t>
+  </si>
+  <si>
+    <t>27B46439844888C8842D5D85C43B843738F91019C97A3D0AC658CF8D845D4674</t>
+  </si>
+  <si>
+    <t>824557834E35F95B0E11225A047DA6D662BF31A4A22A9A066AAC9F0F6797A679</t>
+  </si>
+  <si>
+    <t>AC8FF7817DD343051CD59326DD99BAD1EC58ED33F117F4CA70B2D7D97FBCCCD0</t>
+  </si>
+  <si>
+    <t>02495F5291267F26CB7D7E27FAB853336B92C460717133401E4B5DA4F4691FD9</t>
+  </si>
+  <si>
+    <t>92B097AB201B14C7810BC942E7FA9B1F43F7963650D7FDA35F121C7DE83203B2</t>
+  </si>
+  <si>
+    <t>B3A867656E426EC8E44F008D95E4E347D5E4C84C8E41BD83376B1D9F4251C325</t>
+  </si>
+  <si>
+    <t>654F35A302CAC467D9930086FDA8C8D331850FBE6D3E2C3E17D2498AC35D08CA</t>
+  </si>
+  <si>
+    <t>35789078921B030FDA4BB17C5060EF4CF0A3531065AFB9D9AF709562AF805803</t>
+  </si>
+  <si>
+    <t>53F35395D07C2202CA0CA3DF65AE6B6F65AC811B26C3AE1205C62EE4AD2BE676</t>
+  </si>
+  <si>
+    <t>DFBCCF0B5D451609C9AEE0424818237F19D27CEFE249527E6A84A8F2BAB80FDF</t>
+  </si>
+  <si>
+    <t>B0191A928DDB315F6F4595B4E1D9890622415C90AD099EFEE3F55190C117B2EF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +348,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -264,10 +420,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -283,9 +440,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{72FA8B51-E97A-45D6-B831-061E2FB36BBD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -608,51 +771,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -668,7 +831,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -678,33 +843,558 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -714,33 +1404,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -750,78 +1482,6 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -829,397 +1489,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1249,12 +1564,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1269,7 +1584,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1285,12 +1600,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1388,54 +1703,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1503,10 +1818,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1514,16 +1829,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1554,10 +1869,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1565,16 +1880,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1605,10 +1920,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1616,16 +1931,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1657,10 +1972,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1668,16 +1983,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1693,7 +2008,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,18 +2019,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1730,7 +2045,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1740,18 +2057,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add evidence for B5 to B7
</commit_message>
<xml_diff>
--- a/nurtagum/evidence.xlsx
+++ b/nurtagum/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0K_nurtagum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_ALL_nurtagum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C9FDF-D087-4962-B4C5-EE99485DA1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1C6CEC-7A8B-48D0-8807-B8C656A0A0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="839" firstSheet="5" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="97">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -323,6 +318,24 @@
   </si>
   <si>
     <t>B0191A928DDB315F6F4595B4E1D9890622415C90AD099EFEE3F55190C117B2EF</t>
+  </si>
+  <si>
+    <t>211C3642BAC60BB8FB015D2F2D371B055B43150C1444458C1CDF38AE7B91B7DB</t>
+  </si>
+  <si>
+    <t>5D36596AB5D0B7B33A7918AA17CD95EFCBFE1FD0EF3536C308CEFC60A01E8A47</t>
+  </si>
+  <si>
+    <t>A8294ACE73ECE7983E01E1F09191E169398217CB27AD7946456691B5B011A871</t>
+  </si>
+  <si>
+    <t>B0772DAC28EF560F8E6C7413221EE1982DDB1076F64B28D9B697C6F32A7F9890</t>
+  </si>
+  <si>
+    <t>C32C2BF16C417D6AAB1C5CAD9D5608CE04B979BE0BECE1AC1EAEF19666222812</t>
+  </si>
+  <si>
+    <t>CFB2D9DE5A30D5A85D97A1D58F379526C4065FAEF4CA8B088F3FEF54C130DDFC</t>
   </si>
 </sst>
 </file>
@@ -771,51 +784,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -843,10 +856,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -862,8 +913,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -881,10 +932,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -900,8 +951,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -919,10 +970,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -938,15 +989,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,34 +1008,58 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,55 +1073,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,55 +1135,117 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,55 +1259,154 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>64</v>
+      <c r="A2" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,55 +1420,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,294 +1498,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>74</v>
+      <c r="A3" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1563,6 +1576,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1577,8 +1626,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1600,27 +1649,29 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1634,31 +1685,30 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EBB4D6-7F4F-4887-868B-C2FD618111B7}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1668,12 +1718,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1703,54 +1753,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1818,13 +1868,64 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,29 +1933,29 @@
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,78 +1970,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1972,27 +2022,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2019,18 +2069,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2057,18 +2107,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>